<commit_message>
updated graph with worst case for bmh
</commit_message>
<xml_diff>
--- a/results/AlgorithmsCompared.xlsx
+++ b/results/AlgorithmsCompared.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="161420"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
   <si>
     <t>length of search text</t>
   </si>
@@ -46,12 +46,15 @@
   <si>
     <t>Naïve</t>
   </si>
+  <si>
+    <t>Naive</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,7 +147,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -916,8 +918,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2026895712"/>
-        <c:axId val="-2026895168"/>
+        <c:axId val="597643272"/>
+        <c:axId val="597644040"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1128,7 +1130,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$1</c15:sqref>
@@ -1167,7 +1169,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$2:$A$22</c15:sqref>
@@ -1245,7 +1247,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$2:$C$22</c15:sqref>
@@ -1328,7 +1330,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2026895712"/>
+        <c:axId val="597643272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,7 +1381,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1446,12 +1447,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2026895168"/>
+        <c:crossAx val="597644040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2026895168"/>
+        <c:axId val="597644040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1497,7 +1498,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1564,7 +1564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2026895712"/>
+        <c:crossAx val="597643272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1578,7 +1578,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1685,7 +1684,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2457,8 +2455,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028629968"/>
-        <c:axId val="-2028630512"/>
+        <c:axId val="597662344"/>
+        <c:axId val="597663112"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -2669,7 +2667,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$24</c15:sqref>
@@ -2708,7 +2706,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$25:$A$45</c15:sqref>
@@ -2786,7 +2784,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$25:$C$45</c15:sqref>
@@ -2869,7 +2867,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028629968"/>
+        <c:axId val="597662344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2915,7 +2913,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2982,12 +2979,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2028630512"/>
+        <c:crossAx val="597663112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028630512"/>
+        <c:axId val="597663112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3033,7 +3030,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3100,7 +3096,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2028629968"/>
+        <c:crossAx val="597662344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3114,7 +3110,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3226,7 +3221,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3998,8 +3992,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1994040992"/>
-        <c:axId val="-1994037728"/>
+        <c:axId val="1161479687"/>
+        <c:axId val="1161480455"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -4210,7 +4204,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$47</c15:sqref>
@@ -4249,7 +4243,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$48:$A$68</c15:sqref>
@@ -4327,7 +4321,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$48:$C$68</c15:sqref>
@@ -4410,7 +4404,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1994040992"/>
+        <c:axId val="1161479687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4456,7 +4450,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4523,12 +4516,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1994037728"/>
+        <c:crossAx val="1161480455"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1994037728"/>
+        <c:axId val="1161480455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4574,7 +4567,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4641,7 +4633,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1994040992"/>
+        <c:crossAx val="1161479687"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4655,7 +4647,1130 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algorithms Compared With only New Lines In the File</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$70</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Boyer Moore Horspool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$71:$A$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>419797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>839594</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1259391</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1679188</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2098985</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2518782</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2938579</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3358376</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3778173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4197970</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4617767</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5037564</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5457361</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5877158</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6296955</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6716752</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7136549</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7556346</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7976143</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8395940</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8815737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$71:$D$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>903</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1176</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1468</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1752</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2065</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2356</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2683</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2928</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3219</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3552</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3811</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4123</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4427</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4688</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5019</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5273</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5541</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5862</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6427</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$70</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Knuth Morris Pratt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$71:$A$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>419797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>839594</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1259391</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1679188</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2098985</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2518782</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2938579</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3358376</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3778173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4197970</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4617767</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5037564</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5457361</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5877158</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6296955</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6716752</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7136549</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7556346</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7976143</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8395940</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8815737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$71:$E$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>885</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1082</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1258</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1407</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1614</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1798</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1943</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2166</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2325</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2462</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2720</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2856</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3070</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3256</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3392</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3569</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4806</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$70</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Z</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$71:$A$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>419797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>839594</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1259391</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1679188</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2098985</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2518782</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2938579</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3358376</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3778173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4197970</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4617767</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5037564</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5457361</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5877158</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6296955</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6716752</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7136549</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7556346</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7976143</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8395940</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8815737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$71:$F$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>988</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1237</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1543</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1727</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2082</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2223</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2495</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2731</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2987</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3221</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3426</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3723</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4185</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4672</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4891</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4972</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5558</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$70</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Naive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$71:$A$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>419797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>839594</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1259391</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1679188</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2098985</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2518782</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2938579</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3358376</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3778173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4197970</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4617767</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5037564</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5457361</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5877158</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6296955</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6716752</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7136549</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7556346</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7976143</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8395940</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8815737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$71:$G$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>703</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>881</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1235</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1422</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1529</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1813</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1946</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2317</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2478</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2834</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3057</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3357</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3712</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3764</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1253798279"/>
+        <c:axId val="1253799047"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1253798279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Characters Searched</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1253799047"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1253799047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1253798279"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4842,6 +5957,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6390,24 +7545,546 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>71436</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6425,19 +8102,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6457,7 +8140,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
@@ -6467,7 +8150,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6477,6 +8166,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69C78C81-2E17-4DCD-8704-DCCBE3FA6729}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6748,13 +8473,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -6764,7 +8489,7 @@
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6787,7 +8512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>224361</v>
       </c>
@@ -6810,7 +8535,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>448722</v>
       </c>
@@ -6833,7 +8558,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>673083</v>
       </c>
@@ -6856,7 +8581,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>897444</v>
       </c>
@@ -6879,7 +8604,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>1121805</v>
       </c>
@@ -6902,7 +8627,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>1346166</v>
       </c>
@@ -6925,7 +8650,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>1570527</v>
       </c>
@@ -6948,7 +8673,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>1794888</v>
       </c>
@@ -6971,7 +8696,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>2019249</v>
       </c>
@@ -6994,7 +8719,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>2243610</v>
       </c>
@@ -7017,7 +8742,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>2467971</v>
       </c>
@@ -7040,7 +8765,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>2692332</v>
       </c>
@@ -7063,7 +8788,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>2916693</v>
       </c>
@@ -7086,7 +8811,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>3141054</v>
       </c>
@@ -7109,7 +8834,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>3365415</v>
       </c>
@@ -7132,7 +8857,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>3589776</v>
       </c>
@@ -7155,7 +8880,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>3814137</v>
       </c>
@@ -7178,7 +8903,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>4038498</v>
       </c>
@@ -7201,7 +8926,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>4262859</v>
       </c>
@@ -7224,7 +8949,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>4487220</v>
       </c>
@@ -7247,7 +8972,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>4711581</v>
       </c>
@@ -7270,7 +8995,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -7293,7 +9018,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>224361</v>
       </c>
@@ -7316,7 +9041,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>448722</v>
       </c>
@@ -7339,7 +9064,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>673083</v>
       </c>
@@ -7362,7 +9087,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>897444</v>
       </c>
@@ -7385,7 +9110,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>1121805</v>
       </c>
@@ -7408,7 +9133,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>1346166</v>
       </c>
@@ -7431,7 +9156,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>1570527</v>
       </c>
@@ -7454,7 +9179,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>1794888</v>
       </c>
@@ -7477,7 +9202,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>2019249</v>
       </c>
@@ -7500,7 +9225,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>2243610</v>
       </c>
@@ -7523,7 +9248,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>2467971</v>
       </c>
@@ -7546,7 +9271,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>2692332</v>
       </c>
@@ -7569,7 +9294,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>2916693</v>
       </c>
@@ -7592,7 +9317,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>3141054</v>
       </c>
@@ -7615,7 +9340,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>3365415</v>
       </c>
@@ -7638,7 +9363,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>3589776</v>
       </c>
@@ -7661,7 +9386,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>3814137</v>
       </c>
@@ -7684,7 +9409,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>4038498</v>
       </c>
@@ -7707,7 +9432,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>4262859</v>
       </c>
@@ -7730,7 +9455,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>4487220</v>
       </c>
@@ -7753,7 +9478,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>4711581</v>
       </c>
@@ -7776,7 +9501,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -7799,7 +9524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>224361</v>
       </c>
@@ -7822,7 +9547,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>448722</v>
       </c>
@@ -7845,7 +9570,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>673083</v>
       </c>
@@ -7868,7 +9593,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>897444</v>
       </c>
@@ -7891,7 +9616,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>1121805</v>
       </c>
@@ -7914,7 +9639,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>1346166</v>
       </c>
@@ -7937,7 +9662,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>1570527</v>
       </c>
@@ -7960,7 +9685,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>1794888</v>
       </c>
@@ -7983,7 +9708,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>2019249</v>
       </c>
@@ -8006,7 +9731,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>2243610</v>
       </c>
@@ -8029,7 +9754,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>2467971</v>
       </c>
@@ -8052,7 +9777,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>2692332</v>
       </c>
@@ -8075,7 +9800,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>2916693</v>
       </c>
@@ -8098,7 +9823,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>3141054</v>
       </c>
@@ -8121,7 +9846,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>3365415</v>
       </c>
@@ -8144,7 +9869,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>3589776</v>
       </c>
@@ -8167,7 +9892,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>3814137</v>
       </c>
@@ -8190,7 +9915,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>4038498</v>
       </c>
@@ -8213,7 +9938,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>4262859</v>
       </c>
@@ -8236,7 +9961,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>4487220</v>
       </c>
@@ -8259,7 +9984,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>4711581</v>
       </c>
@@ -8280,6 +10005,512 @@
       </c>
       <c r="G68">
         <v>1218</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" t="s">
+        <v>5</v>
+      </c>
+      <c r="G70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71">
+        <v>419797</v>
+      </c>
+      <c r="B71">
+        <v>21</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>300</v>
+      </c>
+      <c r="E71">
+        <v>184</v>
+      </c>
+      <c r="F71">
+        <v>252</v>
+      </c>
+      <c r="G71">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72">
+        <v>839594</v>
+      </c>
+      <c r="B72">
+        <v>21</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>588</v>
+      </c>
+      <c r="E72">
+        <v>359</v>
+      </c>
+      <c r="F72">
+        <v>521</v>
+      </c>
+      <c r="G72">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73">
+        <v>1259391</v>
+      </c>
+      <c r="B73">
+        <v>21</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>903</v>
+      </c>
+      <c r="E73">
+        <v>590</v>
+      </c>
+      <c r="F73">
+        <v>780</v>
+      </c>
+      <c r="G73">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74">
+        <v>1679188</v>
+      </c>
+      <c r="B74">
+        <v>21</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>1176</v>
+      </c>
+      <c r="E74">
+        <v>713</v>
+      </c>
+      <c r="F74">
+        <v>988</v>
+      </c>
+      <c r="G74">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75">
+        <v>2098985</v>
+      </c>
+      <c r="B75">
+        <v>21</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>1468</v>
+      </c>
+      <c r="E75">
+        <v>885</v>
+      </c>
+      <c r="F75">
+        <v>1237</v>
+      </c>
+      <c r="G75">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76">
+        <v>2518782</v>
+      </c>
+      <c r="B76">
+        <v>21</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>1752</v>
+      </c>
+      <c r="E76">
+        <v>1082</v>
+      </c>
+      <c r="F76">
+        <v>1543</v>
+      </c>
+      <c r="G76">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77">
+        <v>2938579</v>
+      </c>
+      <c r="B77">
+        <v>21</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>2065</v>
+      </c>
+      <c r="E77">
+        <v>1258</v>
+      </c>
+      <c r="F77">
+        <v>1727</v>
+      </c>
+      <c r="G77">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78">
+        <v>3358376</v>
+      </c>
+      <c r="B78">
+        <v>21</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>2356</v>
+      </c>
+      <c r="E78">
+        <v>1407</v>
+      </c>
+      <c r="F78">
+        <v>2082</v>
+      </c>
+      <c r="G78">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79">
+        <v>3778173</v>
+      </c>
+      <c r="B79">
+        <v>21</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>2683</v>
+      </c>
+      <c r="E79">
+        <v>1614</v>
+      </c>
+      <c r="F79">
+        <v>2223</v>
+      </c>
+      <c r="G79">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80">
+        <v>4197970</v>
+      </c>
+      <c r="B80">
+        <v>21</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>2928</v>
+      </c>
+      <c r="E80">
+        <v>1798</v>
+      </c>
+      <c r="F80">
+        <v>2495</v>
+      </c>
+      <c r="G80">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81">
+        <v>4617767</v>
+      </c>
+      <c r="B81">
+        <v>21</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>3219</v>
+      </c>
+      <c r="E81">
+        <v>1943</v>
+      </c>
+      <c r="F81">
+        <v>2731</v>
+      </c>
+      <c r="G81">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82">
+        <v>5037564</v>
+      </c>
+      <c r="B82">
+        <v>21</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>3552</v>
+      </c>
+      <c r="E82">
+        <v>2166</v>
+      </c>
+      <c r="F82">
+        <v>2987</v>
+      </c>
+      <c r="G82">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83">
+        <v>5457361</v>
+      </c>
+      <c r="B83">
+        <v>21</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>3811</v>
+      </c>
+      <c r="E83">
+        <v>2325</v>
+      </c>
+      <c r="F83">
+        <v>3221</v>
+      </c>
+      <c r="G83">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84">
+        <v>5877158</v>
+      </c>
+      <c r="B84">
+        <v>21</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>4123</v>
+      </c>
+      <c r="E84">
+        <v>2462</v>
+      </c>
+      <c r="F84">
+        <v>3426</v>
+      </c>
+      <c r="G84">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85">
+        <v>6296955</v>
+      </c>
+      <c r="B85">
+        <v>21</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>4427</v>
+      </c>
+      <c r="E85">
+        <v>2720</v>
+      </c>
+      <c r="F85">
+        <v>3723</v>
+      </c>
+      <c r="G85">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86">
+        <v>6716752</v>
+      </c>
+      <c r="B86">
+        <v>21</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>4688</v>
+      </c>
+      <c r="E86">
+        <v>2856</v>
+      </c>
+      <c r="F86">
+        <v>3995</v>
+      </c>
+      <c r="G86">
+        <v>2834</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87">
+        <v>7136549</v>
+      </c>
+      <c r="B87">
+        <v>21</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>5019</v>
+      </c>
+      <c r="E87">
+        <v>3070</v>
+      </c>
+      <c r="F87">
+        <v>4185</v>
+      </c>
+      <c r="G87">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88">
+        <v>7556346</v>
+      </c>
+      <c r="B88">
+        <v>21</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>5273</v>
+      </c>
+      <c r="E88">
+        <v>3256</v>
+      </c>
+      <c r="F88">
+        <v>4672</v>
+      </c>
+      <c r="G88">
+        <v>3057</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89">
+        <v>7976143</v>
+      </c>
+      <c r="B89">
+        <v>21</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>5541</v>
+      </c>
+      <c r="E89">
+        <v>3392</v>
+      </c>
+      <c r="F89">
+        <v>4891</v>
+      </c>
+      <c r="G89">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90">
+        <v>8395940</v>
+      </c>
+      <c r="B90">
+        <v>21</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>5862</v>
+      </c>
+      <c r="E90">
+        <v>3569</v>
+      </c>
+      <c r="F90">
+        <v>4972</v>
+      </c>
+      <c r="G90">
+        <v>3712</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91">
+        <v>8815737</v>
+      </c>
+      <c r="B91">
+        <v>21</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>6427</v>
+      </c>
+      <c r="E91">
+        <v>4806</v>
+      </c>
+      <c r="F91">
+        <v>5558</v>
+      </c>
+      <c r="G91">
+        <v>3764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>